<commit_message>
db backup and restore
</commit_message>
<xml_diff>
--- a/registeration.xlsx
+++ b/registeration.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N24"/>
+  <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -508,17 +508,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>01555250555</t>
+          <t>01555250000</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>محمد</t>
+          <t>علي</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>زيادة</t>
+          <t>السديس</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -528,32 +528,28 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>محمود</t>
+          <t>كمال</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>إبراهيم</t>
+          <t>أيمن</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>زيادة</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>قريب</t>
-        </is>
-      </c>
+          <t>الجوهري</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr">
         <is>
-          <t>من 20 سنة حتى 50 سنة</t>
+          <t>أقل من 19 سنة</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>ذكر</t>
+          <t>أنثى</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -569,136 +565,72 @@
       <c r="M2" t="inlineStr"/>
       <c r="N2" t="inlineStr">
         <is>
-          <t>528</t>
+          <t>515</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>01555250000</t>
+          <t>+1-271-862-3226x9596</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>علي</t>
+          <t>Cindy</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>السديس</t>
+          <t>Davis</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>أحمد</t>
+          <t>Marquez</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>كمال</t>
+          <t>Crawford</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>أيمن</t>
+          <t>Fleming</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>الجوهري</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr"/>
+          <t>Hutchinson</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>might</t>
+        </is>
+      </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>أقل من 19 سنة</t>
+          <t>من 20 سنة حتى 50 سنة</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>أنثى</t>
+          <t>ذكر</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>القاهرة</t>
+          <t>North Samanthashire</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>سوف أحضر باذن الله</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr"/>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>515</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>+1-271-862-3226x9596</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Cindy</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Davis</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Marquez</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Crawford</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Fleming</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>Hutchinson</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>might</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>من 20 سنة حتى 50 سنة</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>ذكر</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>North Samanthashire</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
           <t>أعتذر عن الحضور</t>
         </is>
       </c>
-      <c r="M4" t="inlineStr">
+      <c r="M3" t="inlineStr">
         <is>
           <t>Security opportunity school just back.
 Herself culture term trade.
@@ -706,21 +638,93 @@
 Central other away. Family report soldier tree.</t>
         </is>
       </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>146</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>(721)612-9815</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Brittany</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Thompson</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Williams</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Mooney</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Herrera</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Shelton</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>lay</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>من 20 سنة حتى 50 سنة</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>أنثى</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>Kevinfurt</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>سوف أحضر باذن الله</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>Air wide suggest hope everybody manager. Administration alone attorney information first sometimes however. Trip song dog. Each boy north become.</t>
+        </is>
+      </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>146</t>
+          <t>998</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>647-658-3847</t>
+          <t>553.434.3463x9855</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Michael</t>
+          <t>Stephen</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -730,142 +734,143 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Gonzales</t>
+          <t>Woods</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Carlson</t>
+          <t>Myers</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Rosales</t>
+          <t>Gonzalez</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Middleton</t>
+          <t>Chaney</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>either</t>
+          <t>son</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>أقل من 19 سنة</t>
+          <t>من 20 سنة حتى 50 سنة</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>ذكر</t>
+          <t>أنثى</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>Matthewville</t>
+          <t>Stephenburgh</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>سوف أحضر باذن الله</t>
+          <t>أعتذر عن الحضور</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>Pattern focus again federal money particular war.
-Understand final open couple recently here next. Alone prevent guy go reality remember school.</t>
+          <t>Where able difficult information ten. Right hope operation bed behavior of recent.
+Get thank national. Then still example improve. Couple join material poor inside until he.</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>109</t>
+          <t>530</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>(721)612-9815</t>
+          <t>(774)689-3101x918</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Brittany</t>
+          <t>Eric</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Thompson</t>
+          <t>Johnson</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Williams</t>
+          <t>Armstrong</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Mooney</t>
+          <t>Hartman</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Herrera</t>
+          <t>Cox</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Shelton</t>
+          <t>Brown</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>lay</t>
+          <t>argue</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>من 20 سنة حتى 50 سنة</t>
+          <t>أقل من 19 سنة</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>أنثى</t>
+          <t>ذكر</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>Kevinfurt</t>
+          <t>Brownland</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>سوف أحضر باذن الله</t>
+          <t>أعتذر عن الحضور</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>Air wide suggest hope everybody manager. Administration alone attorney information first sometimes however. Trip song dog. Each boy north become.</t>
+          <t>Organization during player trade real effect enough. Chair writer decision save technology big among stand. Choose stay like become mother.
+Point security fill catch.</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>998</t>
+          <t>854</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>553.434.3463x9855</t>
+          <t>(391)952-6930x094</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Stephen</t>
+          <t>Rachael</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -875,27 +880,27 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Woods</t>
+          <t>Thompson</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Myers</t>
+          <t>Beck</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Gonzalez</t>
+          <t>Walker</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Chaney</t>
+          <t>Byrd</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>son</t>
+          <t>might</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
@@ -905,85 +910,85 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>أنثى</t>
+          <t>ذكر</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>Stephenburgh</t>
+          <t>Nunezhaven</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>أعتذر عن الحضور</t>
+          <t>سوف أحضر باذن الله</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>Where able difficult information ten. Right hope operation bed behavior of recent.
-Get thank national. Then still example improve. Couple join material poor inside until he.</t>
+          <t>Exactly to area early development purpose focus local. Cut attorney understand power side send.</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>530</t>
+          <t>446</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>(774)689-3101x918</t>
+          <t>532.574.7317</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Eric</t>
+          <t>Laura</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Johnson</t>
+          <t>Mills</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Armstrong</t>
+          <t>Freeman</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Hartman</t>
+          <t>Thomas</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Cox</t>
+          <t>Henry</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Brown</t>
+          <t>Campbell</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>argue</t>
+          <t>range</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>أقل من 19 سنة</t>
+          <t xml:space="preserve">من 20 سنة حتى 50 سنة
+</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>ذكر</t>
+          <t>أنثى</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>Brownland</t>
+          <t>Christopherland</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
@@ -993,143 +998,143 @@
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>Organization during player trade real effect enough. Chair writer decision save technology big among stand. Choose stay like become mother.
-Point security fill catch.</t>
+          <t>Practice hope notice event author lay. Month air no dream eye. Cell industry page her federal often. Easy back few exactly not with.
+Reality vote conference this after thousand property.</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>854</t>
+          <t>194</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>(391)952-6930x094</t>
+          <t>(336)434-6038</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Rachael</t>
+          <t>Nicole</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>السديس</t>
+          <t>James</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Thompson</t>
+          <t>Campbell</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Beck</t>
+          <t>Ferguson</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Walker</t>
+          <t>Barron</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Byrd</t>
+          <t>Price</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>might</t>
+          <t>different</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>من 20 سنة حتى 50 سنة</t>
+          <t>أقل من 19 سنة</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>ذكر</t>
+          <t>أنثى</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>Nunezhaven</t>
+          <t>Shermanberg</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>سوف أحضر باذن الله</t>
+          <t>أعتذر عن الحضور</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>Exactly to area early development purpose focus local. Cut attorney understand power side send.</t>
+          <t>Economy structure keep herself fast eight agree thing. Vote of west receive last change. Amount general effect.
+Without yet financial hard yeah. Size on increase responsibility concern thus baby.</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>446</t>
+          <t>320</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>532.574.7317</t>
+          <t>924.663.1287x96198</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Laura</t>
+          <t>Kelly</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Mills</t>
+          <t>Zavala</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Freeman</t>
+          <t>Snyder</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Thomas</t>
+          <t>Thompson</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Henry</t>
+          <t>Davis</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Campbell</t>
+          <t>Smith</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>range</t>
+          <t>hear</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t xml:space="preserve">من 20 سنة حتى 50 سنة
-</t>
+          <t>48</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>أنثى</t>
+          <t>ذكر</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>Christopherland</t>
+          <t>Davisville</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
@@ -1139,143 +1144,142 @@
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>Practice hope notice event author lay. Month air no dream eye. Cell industry page her federal often. Easy back few exactly not with.
-Reality vote conference this after thousand property.</t>
+          <t>Physical morning design push adult daughter. Official western training artist.
+Institution bad final commercial good others something. Enter newspaper laugh lot.</t>
         </is>
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>194</t>
+          <t>373</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>(336)434-6038</t>
+          <t>639-290-6636x2786</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Nicole</t>
+          <t>Annette</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>James</t>
+          <t>Mendoza</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Campbell</t>
+          <t>Macias</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Ferguson</t>
+          <t>Lang</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Barron</t>
+          <t>Peterson</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Price</t>
+          <t>Ortiz</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>different</t>
+          <t>where</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>أقل من 19 سنة</t>
+          <t>23</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>أنثى</t>
+          <t>ذكر</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>Shermanberg</t>
+          <t>Rebeccaburgh</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>أعتذر عن الحضور</t>
+          <t>سوف أحضر باذن الله</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>Economy structure keep herself fast eight agree thing. Vote of west receive last change. Amount general effect.
-Without yet financial hard yeah. Size on increase responsibility concern thus baby.</t>
+          <t>Against control mother people sea heart second. Enter prepare throw health family by every.</t>
         </is>
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>320</t>
+          <t>682</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>924.663.1287x96198</t>
+          <t>362-486-5142x258</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Kelly</t>
+          <t>Jacob</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Zavala</t>
+          <t>Zimmerman</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Snyder</t>
+          <t>Hart</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Thompson</t>
+          <t>Reyes</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Davis</t>
+          <t>Johnson</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Smith</t>
+          <t>Powell</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>hear</t>
+          <t>become</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>48</t>
+          <t>26</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>ذكر</t>
+          <t>أنثى</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>Davisville</t>
+          <t>East Maryton</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
@@ -1285,132 +1289,133 @@
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>Physical morning design push adult daughter. Official western training artist.
-Institution bad final commercial good others something. Enter newspaper laugh lot.</t>
+          <t>Ever national television position something election. Now yard down account thought according major.
+Above fly young little. Trade trade respond before church.</t>
         </is>
       </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t>373</t>
+          <t>634</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>639-290-6636x2786</t>
+          <t>+1-415-235-1666x739</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Annette</t>
+          <t>Eric</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Mendoza</t>
+          <t>Cunningham</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Macias</t>
+          <t>Roman</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Lang</t>
+          <t>Reid</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Peterson</t>
+          <t>Poole</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Ortiz</t>
+          <t>Kelly</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>where</t>
+          <t>mean</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>30</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>ذكر</t>
+          <t>أنثى</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>Rebeccaburgh</t>
+          <t>West Brian</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>سوف أحضر باذن الله</t>
+          <t>أعتذر عن الحضور</t>
         </is>
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>Against control mother people sea heart second. Enter prepare throw health family by every.</t>
+          <t>Board financial threat hit ask investment. Cost hit him myself.
+What natural defense air official magazine. Much appear drug growth human high make.</t>
         </is>
       </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t>682</t>
+          <t>290</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>362-486-5142x258</t>
+          <t>+1-528-305-2614x97014</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Jacob</t>
+          <t>Jeremy</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Zimmerman</t>
+          <t>Perez</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Hart</t>
+          <t>Adams</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Reyes</t>
+          <t>Curtis</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Johnson</t>
+          <t>Chambers</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Powell</t>
+          <t>Davis</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>become</t>
+          <t>feel</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>26</t>
+          <t>22</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
@@ -1420,7 +1425,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>East Maryton</t>
+          <t>Millerview</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
@@ -1430,133 +1435,133 @@
       </c>
       <c r="M14" t="inlineStr">
         <is>
-          <t>Ever national television position something election. Now yard down account thought according major.
-Above fly young little. Trade trade respond before church.</t>
+          <t>Realize community beautiful receive account use back. Floor religious around two my.
+Natural action data. Live get something project station even.</t>
         </is>
       </c>
       <c r="N14" t="inlineStr">
         <is>
-          <t>634</t>
+          <t>693</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>+1-415-235-1666x739</t>
+          <t>5637916431</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Eric</t>
+          <t>Allison</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Cunningham</t>
+          <t>Taylor</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Roman</t>
+          <t>Hartman</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Reid</t>
+          <t>Lane</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Poole</t>
+          <t>Anderson</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Kelly</t>
+          <t>Yoder</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>mean</t>
+          <t>compare</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>74</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>أنثى</t>
+          <t>ذكر</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>West Brian</t>
+          <t>South Thomas</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>أعتذر عن الحضور</t>
+          <t>سوف أحضر باذن الله</t>
         </is>
       </c>
       <c r="M15" t="inlineStr">
         <is>
-          <t>Board financial threat hit ask investment. Cost hit him myself.
-What natural defense air official magazine. Much appear drug growth human high make.</t>
+          <t>Standard ten above final save always particular member. So maybe outside institution. Loss few vote environment.
+Upon old try wife. Expert physical development national surface social.</t>
         </is>
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>290</t>
+          <t>671</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>+1-528-305-2614x97014</t>
+          <t>891.472.6565x40491</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Jeremy</t>
+          <t>Daniel</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Perez</t>
+          <t>Jones</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Adams</t>
+          <t>Cannon</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Curtis</t>
+          <t>Gonzalez</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Chambers</t>
+          <t>Brown</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Davis</t>
+          <t>Smith</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>feel</t>
+          <t>such</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>30</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
@@ -1566,80 +1571,80 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>Millerview</t>
+          <t>Hendersonview</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>أعتذر عن الحضور</t>
+          <t>سوف أحضر باذن الله</t>
         </is>
       </c>
       <c r="M16" t="inlineStr">
         <is>
-          <t>Realize community beautiful receive account use back. Floor religious around two my.
-Natural action data. Live get something project station even.</t>
+          <t>Ground those others throw a goal reach remember. Approach effect stop work treat continue bill character. Myself act behind those.
+Garden those plan mind day well increase wall.</t>
         </is>
       </c>
       <c r="N16" t="inlineStr">
         <is>
-          <t>693</t>
+          <t>393</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>5637916431</t>
+          <t>+1-660-804-9714x112</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Allison</t>
+          <t>Ronald</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Taylor</t>
+          <t>Rodgers</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Hartman</t>
+          <t>Warren</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Lane</t>
+          <t>Reilly</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Anderson</t>
+          <t>Garcia</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Yoder</t>
+          <t>Barnes</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>compare</t>
+          <t>artist</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>74</t>
+          <t>63</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>ذكر</t>
+          <t>أنثى</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>South Thomas</t>
+          <t>Fletcherfurt</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
@@ -1649,60 +1654,59 @@
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>Standard ten above final save always particular member. So maybe outside institution. Loss few vote environment.
-Upon old try wife. Expert physical development national surface social.</t>
+          <t>Space from piece include read could. Century everything couple yeah remember after step least. Family fund simply often growth.</t>
         </is>
       </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t>671</t>
+          <t>578</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>891.472.6565x40491</t>
+          <t>438-821-6154</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Daniel</t>
+          <t>Antonio</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Jones</t>
+          <t>Cooke</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Cannon</t>
+          <t>Spence</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Gonzalez</t>
+          <t>Flynn</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Brown</t>
+          <t>Moore</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Smith</t>
+          <t>Hall</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>such</t>
+          <t>by</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>80</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
@@ -1712,160 +1716,15 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>Hendersonview</t>
+          <t>New Kathleen</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>سوف أحضر باذن الله</t>
+          <t>أعتذر عن الحضور</t>
         </is>
       </c>
       <c r="M18" t="inlineStr">
-        <is>
-          <t>Ground those others throw a goal reach remember. Approach effect stop work treat continue bill character. Myself act behind those.
-Garden those plan mind day well increase wall.</t>
-        </is>
-      </c>
-      <c r="N18" t="inlineStr">
-        <is>
-          <t>393</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>+1-660-804-9714x112</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>Ronald</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>Rodgers</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>Warren</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>Reilly</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>Garcia</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>Barnes</t>
-        </is>
-      </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>artist</t>
-        </is>
-      </c>
-      <c r="I19" t="inlineStr">
-        <is>
-          <t>63</t>
-        </is>
-      </c>
-      <c r="J19" t="inlineStr">
-        <is>
-          <t>أنثى</t>
-        </is>
-      </c>
-      <c r="K19" t="inlineStr">
-        <is>
-          <t>Fletcherfurt</t>
-        </is>
-      </c>
-      <c r="L19" t="inlineStr">
-        <is>
-          <t>سوف أحضر باذن الله</t>
-        </is>
-      </c>
-      <c r="M19" t="inlineStr">
-        <is>
-          <t>Space from piece include read could. Century everything couple yeah remember after step least. Family fund simply often growth.</t>
-        </is>
-      </c>
-      <c r="N19" t="inlineStr">
-        <is>
-          <t>578</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>438-821-6154</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>Antonio</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>Cooke</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>Spence</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>Flynn</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>Moore</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>Hall</t>
-        </is>
-      </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>by</t>
-        </is>
-      </c>
-      <c r="I20" t="inlineStr">
-        <is>
-          <t>80</t>
-        </is>
-      </c>
-      <c r="J20" t="inlineStr">
-        <is>
-          <t>أنثى</t>
-        </is>
-      </c>
-      <c r="K20" t="inlineStr">
-        <is>
-          <t>New Kathleen</t>
-        </is>
-      </c>
-      <c r="L20" t="inlineStr">
-        <is>
-          <t>أعتذر عن الحضور</t>
-        </is>
-      </c>
-      <c r="M20" t="inlineStr">
         <is>
           <t>Leg no leg know.
 About happy speak agent. Cultural crime scene picture teacher least operation.
@@ -1873,16 +1732,144 @@
 Despite baby challenge.</t>
         </is>
       </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>991</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>01555250554</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>محمد</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>السديس</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>أحمد</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>محمود</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>إبراهيم</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>زيادة</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr"/>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>أقل من 19 سنة</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>ذكر</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>القاهرة</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>سوف أحضر باذن الله</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr"/>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>641</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>01555250553</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>علي</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>السديس</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>أحمد</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>كمال</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>إبراهيم</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>علي</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr"/>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>أقل من 19 سنة</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>ذكر</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>القاهرة</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>سوف أحضر باذن الله</t>
+        </is>
+      </c>
+      <c r="M20" t="inlineStr"/>
       <c r="N20" t="inlineStr">
         <is>
-          <t>991</t>
+          <t>790</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>01555250554</t>
+          <t>01555250505</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1912,7 +1899,7 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>زيادة</t>
+          <t>علي</t>
         </is>
       </c>
       <c r="H21" t="inlineStr"/>
@@ -1939,19 +1926,19 @@
       <c r="M21" t="inlineStr"/>
       <c r="N21" t="inlineStr">
         <is>
-          <t>641</t>
+          <t>423</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>01555250553</t>
+          <t>0555618871</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>علي</t>
+          <t>ساره</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1961,38 +1948,38 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>أحمد</t>
+          <t>عمر</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>كمال</t>
+          <t>عبدالله</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>إبراهيم</t>
+          <t>سليمان</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>علي</t>
+          <t>عبدالله</t>
         </is>
       </c>
       <c r="H22" t="inlineStr"/>
       <c r="I22" t="inlineStr">
         <is>
-          <t>أقل من 19 سنة</t>
+          <t>من 20 سنة حتى 50 سنة</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>ذكر</t>
+          <t>أنثى</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>القاهرة</t>
+          <t>الرياض</t>
         </is>
       </c>
       <c r="L22" t="inlineStr">
@@ -2002,134 +1989,6 @@
       </c>
       <c r="M22" t="inlineStr"/>
       <c r="N22" t="inlineStr">
-        <is>
-          <t>790</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>01555250505</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>محمد</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>السديس</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>أحمد</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>محمود</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>إبراهيم</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>علي</t>
-        </is>
-      </c>
-      <c r="H23" t="inlineStr"/>
-      <c r="I23" t="inlineStr">
-        <is>
-          <t>أقل من 19 سنة</t>
-        </is>
-      </c>
-      <c r="J23" t="inlineStr">
-        <is>
-          <t>ذكر</t>
-        </is>
-      </c>
-      <c r="K23" t="inlineStr">
-        <is>
-          <t>القاهرة</t>
-        </is>
-      </c>
-      <c r="L23" t="inlineStr">
-        <is>
-          <t>سوف أحضر باذن الله</t>
-        </is>
-      </c>
-      <c r="M23" t="inlineStr"/>
-      <c r="N23" t="inlineStr">
-        <is>
-          <t>423</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>0555618871</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>ساره</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>السديس</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>عمر</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>عبدالله</t>
-        </is>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>سليمان</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>عبدالله</t>
-        </is>
-      </c>
-      <c r="H24" t="inlineStr"/>
-      <c r="I24" t="inlineStr">
-        <is>
-          <t>من 20 سنة حتى 50 سنة</t>
-        </is>
-      </c>
-      <c r="J24" t="inlineStr">
-        <is>
-          <t>أنثى</t>
-        </is>
-      </c>
-      <c r="K24" t="inlineStr">
-        <is>
-          <t>الرياض</t>
-        </is>
-      </c>
-      <c r="L24" t="inlineStr">
-        <is>
-          <t>سوف أحضر باذن الله</t>
-        </is>
-      </c>
-      <c r="M24" t="inlineStr"/>
-      <c r="N24" t="inlineStr">
         <is>
           <t>157</t>
         </is>

</xml_diff>